<commit_message>
Updated system test 5.0.0 results
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_results/Release_5.0.0_manual_system_tests_outcome_September_2018.xlsx
+++ b/testing/manual_system_tests_results/Release_5.0.0_manual_system_tests_outcome_September_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dzd77598\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Instrument\Dev\ibex_developers_manual.wiki\testing\manual_system_tests_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockStructure="1"/>
@@ -21,24 +21,25 @@
   </sheets>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Potter, Rory (-,RAL,ISIS) - Personal View" guid="{984FFA58-0E1E-44C9-A906-B9154475911A}" mergeInterval="0" personalView="1" xWindow="163" yWindow="95" windowWidth="1440" windowHeight="1014" activeSheetId="3"/>
+    <customWorkbookView name="Liam - Personal View" guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Spencer, Jeremy (STFC,RAL,SC) - Personal View" guid="{3C568D49-0283-4011-B94D-E411C6036403}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1928" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="2"/>
+    <customWorkbookView name="Potter, Adrian (Tessella,RAL,ISIS) - Personal View" guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1014" activeSheetId="2"/>
+    <customWorkbookView name="Oram, Dominic (STFC,RAL,ISIS) - Personal View" guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="894" activeSheetId="2"/>
+    <customWorkbookView name="Akeroyd, Freddie (STFC,RAL,ISIS) - Personal View" guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1667" windowHeight="917" activeSheetId="2"/>
+    <customWorkbookView name="David Keymer - Personal View" guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1789" windowHeight="772" activeSheetId="2"/>
+    <customWorkbookView name="Willemsen, Thomas (Tessella,RAL,ISIS) - Personal View" guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="2"/>
+    <customWorkbookView name="Clarke, Matt (STFC,RAL,ISIS) - Personal View" guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" mergeInterval="0" personalView="1" xWindow="75" yWindow="75" windowWidth="1707" windowHeight="1032" activeSheetId="2"/>
+    <customWorkbookView name="Kathryn Baker - Personal View" guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="2"/>
+    <customWorkbookView name="Baker, Kathryn (STFC,RAL,ISIS) - Personal View" guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="2"/>
+    <customWorkbookView name="Lohnert, Thomas (STFC,RAL,ISIS) - Personal View" guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="974" activeSheetId="3"/>
     <customWorkbookView name="Holt, John (Tessella,RAL,ISIS) - Personal View" guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" autoUpdate="1" mergeInterval="5" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1186" activeSheetId="1"/>
-    <customWorkbookView name="Lohnert, Thomas (STFC,RAL,ISIS) - Personal View" guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="974" activeSheetId="3"/>
-    <customWorkbookView name="Baker, Kathryn (STFC,RAL,ISIS) - Personal View" guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="2"/>
-    <customWorkbookView name="Kathryn Baker - Personal View" guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="2"/>
-    <customWorkbookView name="Clarke, Matt (STFC,RAL,ISIS) - Personal View" guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" mergeInterval="0" personalView="1" xWindow="75" yWindow="75" windowWidth="1707" windowHeight="1032" activeSheetId="2"/>
-    <customWorkbookView name="Willemsen, Thomas (Tessella,RAL,ISIS) - Personal View" guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="2"/>
-    <customWorkbookView name="David Keymer - Personal View" guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1789" windowHeight="772" activeSheetId="2"/>
-    <customWorkbookView name="Akeroyd, Freddie (STFC,RAL,ISIS) - Personal View" guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1667" windowHeight="917" activeSheetId="2"/>
-    <customWorkbookView name="Oram, Dominic (STFC,RAL,ISIS) - Personal View" guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="894" activeSheetId="2"/>
-    <customWorkbookView name="Potter, Adrian (Tessella,RAL,ISIS) - Personal View" guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1014" activeSheetId="2"/>
-    <customWorkbookView name="Spencer, Jeremy (STFC,RAL,SC) - Personal View" guid="{3C568D49-0283-4011-B94D-E411C6036403}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1928" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="2"/>
-    <customWorkbookView name="Liam - Personal View" guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="454">
   <si>
     <t>Test Number</t>
   </si>
@@ -1415,6 +1416,15 @@
   </si>
   <si>
     <t xml:space="preserve">Ticket for release </t>
+  </si>
+  <si>
+    <t>Can't delete a synoptic</t>
+  </si>
+  <si>
+    <t>Keyboard shortcuts don't work</t>
+  </si>
+  <si>
+    <t>rcptt_synoptics are added to repo</t>
   </si>
 </sst>
 </file>
@@ -1978,6 +1988,38 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2011,38 +2053,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2677,7 +2687,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B3DF8C78-20A7-4668-AD63-902129467E1D}" diskRevisions="1" revisionId="880" version="7">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A59EE6FF-4FE2-44AA-B11A-0E04B0BB8A41}" diskRevisions="1" revisionId="886" version="8">
   <header guid="{FDC6F7DD-E568-4A37-A0D9-A34770F1FA09}" dateTime="2018-08-30T11:40:37" maxSheetId="6" userName="Liam" r:id="rId52">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -2759,12 +2769,68 @@
       <sheetId val="5"/>
     </sheetIdMap>
   </header>
+  <header guid="{A59EE6FF-4FE2-44AA-B11A-0E04B0BB8A41}" dateTime="2018-09-17T15:04:55" maxSheetId="6" userName="Potter, Rory (-,RAL,ISIS)" r:id="rId61" minRId="881" maxRId="886">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="881" sId="3" odxf="1">
+    <nc r="C4">
+      <v>3488</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="882" sId="3" odxf="1">
+    <nc r="D4" t="inlineStr">
+      <is>
+        <t>Can't delete a synoptic</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="883" sId="3" odxf="1">
+    <nc r="C5">
+      <v>3548</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="884" sId="3" odxf="1">
+    <nc r="D5" t="inlineStr">
+      <is>
+        <t>Keyboard shortcuts don't work</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="885" sId="3" odxf="1">
+    <nc r="C7">
+      <v>3549</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="886" sId="3">
+    <nc r="D7" t="inlineStr">
+      <is>
+        <t>rcptt_synoptics are added to repo</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{984FFA58-0E1E-44C9-A906-B9154475911A}" action="add"/>
 </revisions>
 </file>
 
@@ -12622,7 +12688,7 @@
         <v>57</v>
       </c>
       <c r="J18" s="8"/>
-      <c r="K18" s="106" t="s">
+      <c r="K18" s="93" t="s">
         <v>360</v>
       </c>
       <c r="L18" s="8"/>
@@ -13940,7 +14006,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="3" t="str">
-        <f t="shared" ref="C38:C69" si="2">CONCATENATE(A63,"-",B63)</f>
+        <f t="shared" ref="C63:C69" si="2">CONCATENATE(A63,"-",B63)</f>
         <v>30-1</v>
       </c>
       <c r="D63" s="20"/>
@@ -14207,10 +14273,10 @@
       <c r="G71" s="50" t="s">
         <v>199</v>
       </c>
-      <c r="H71" s="109" t="s">
+      <c r="H71" s="96" t="s">
         <v>354</v>
       </c>
-      <c r="I71" s="110" t="s">
+      <c r="I71" s="97" t="s">
         <v>408</v>
       </c>
       <c r="J71" s="82" t="s">
@@ -14296,29 +14362,34 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" topLeftCell="A28">
-      <selection activeCell="L34" sqref="L34"/>
+    <customSheetView guid="{984FFA58-0E1E-44C9-A906-B9154475911A}" topLeftCell="A64">
+      <selection activeCell="I48" sqref="I48"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}" topLeftCell="A10">
-      <selection activeCell="K25" sqref="K25"/>
+    <customSheetView guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}" topLeftCell="A10">
+      <selection activeCell="L33" sqref="L33"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" topLeftCell="A58">
-      <selection activeCell="H15" sqref="H15"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{3C568D49-0283-4011-B94D-E411C6036403}" topLeftCell="A64">
       <selection activeCell="I70" sqref="I70"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}" topLeftCell="A10">
-      <selection activeCell="L33" sqref="L33"/>
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" topLeftCell="A58">
+      <selection activeCell="H15" sqref="H15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}" topLeftCell="A10">
+      <selection activeCell="K25" sqref="K25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+    </customSheetView>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" topLeftCell="A28">
+      <selection activeCell="L34" sqref="L34"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="K33:K69 K10:K30">
@@ -14412,7 +14483,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -14441,7 +14512,7 @@
     <col min="13" max="13" width="57.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="56.25">
+    <row r="1" spans="1:13" ht="57">
       <c r="A1" s="17" t="s">
         <v>175</v>
       </c>
@@ -14720,7 +14791,7 @@
       <c r="K9" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="L9" s="100" t="s">
+      <c r="L9" s="118" t="s">
         <v>312</v>
       </c>
       <c r="M9" s="6"/>
@@ -14752,7 +14823,7 @@
       <c r="K10" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="L10" s="101"/>
+      <c r="L10" s="119"/>
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" ht="15">
@@ -14782,7 +14853,7 @@
       <c r="K11" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="L11" s="101"/>
+      <c r="L11" s="119"/>
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" ht="15">
@@ -14812,7 +14883,7 @@
       <c r="K12" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="L12" s="101"/>
+      <c r="L12" s="119"/>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" ht="15">
@@ -14842,7 +14913,7 @@
       <c r="K13" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="L13" s="101"/>
+      <c r="L13" s="119"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" ht="60">
@@ -15420,7 +15491,7 @@
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="111" t="s">
+      <c r="F32" s="98" t="s">
         <v>52</v>
       </c>
       <c r="G32" s="9" t="s">
@@ -17008,7 +17079,7 @@
         <v>64</v>
       </c>
       <c r="C85" s="3" t="str">
-        <f t="shared" ref="C69:C100" si="2">CONCATENATE(A85,"-",B85)</f>
+        <f t="shared" ref="C85:C100" si="2">CONCATENATE(A85,"-",B85)</f>
         <v>15-64</v>
       </c>
       <c r="D85" s="38"/>
@@ -17725,7 +17796,7 @@
       <c r="K108" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="L108" s="102" t="s">
+      <c r="L108" s="120" t="s">
         <v>373</v>
       </c>
     </row>
@@ -17756,7 +17827,7 @@
       <c r="K109" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="L109" s="103"/>
+      <c r="L109" s="121"/>
       <c r="M109" s="6"/>
     </row>
     <row r="110" spans="1:13" ht="45">
@@ -17788,7 +17859,7 @@
       <c r="K110" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="L110" s="103"/>
+      <c r="L110" s="121"/>
       <c r="M110" s="6"/>
     </row>
     <row r="111" spans="1:13" ht="30">
@@ -17818,7 +17889,7 @@
       <c r="K111" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="L111" s="104"/>
+      <c r="L111" s="122"/>
       <c r="M111" s="6"/>
     </row>
     <row r="112" spans="1:13" ht="26.25">
@@ -17828,23 +17899,23 @@
       <c r="B112">
         <v>2</v>
       </c>
-      <c r="C112" s="114" t="s">
+      <c r="C112" s="101" t="s">
         <v>437</v>
       </c>
-      <c r="D112" s="117"/>
-      <c r="E112" s="117"/>
-      <c r="F112" s="117"/>
-      <c r="G112" s="115" t="s">
+      <c r="D112" s="104"/>
+      <c r="E112" s="104"/>
+      <c r="F112" s="104"/>
+      <c r="G112" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="H112" s="115" t="s">
+      <c r="H112" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="I112" s="116" t="s">
+      <c r="I112" s="103" t="s">
         <v>163</v>
       </c>
-      <c r="J112" s="116"/>
-      <c r="K112" s="115" t="s">
+      <c r="J112" s="103"/>
+      <c r="K112" s="102" t="s">
         <v>360</v>
       </c>
       <c r="L112" s="12"/>
@@ -17857,23 +17928,23 @@
       <c r="B113">
         <v>3</v>
       </c>
-      <c r="C113" s="114" t="s">
+      <c r="C113" s="101" t="s">
         <v>438</v>
       </c>
-      <c r="D113" s="117"/>
-      <c r="E113" s="117"/>
-      <c r="F113" s="117"/>
-      <c r="G113" s="115" t="s">
+      <c r="D113" s="104"/>
+      <c r="E113" s="104"/>
+      <c r="F113" s="104"/>
+      <c r="G113" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="H113" s="115" t="s">
+      <c r="H113" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="I113" s="116" t="s">
+      <c r="I113" s="103" t="s">
         <v>164</v>
       </c>
-      <c r="J113" s="116"/>
-      <c r="K113" s="115" t="s">
+      <c r="J113" s="103"/>
+      <c r="K113" s="102" t="s">
         <v>360</v>
       </c>
       <c r="L113" s="12" t="s">
@@ -17888,21 +17959,21 @@
       <c r="B114">
         <v>6</v>
       </c>
-      <c r="C114" s="114" t="s">
+      <c r="C114" s="101" t="s">
         <v>439</v>
       </c>
-      <c r="D114" s="118"/>
-      <c r="E114" s="118"/>
-      <c r="F114" s="118"/>
-      <c r="G114" s="119"/>
-      <c r="H114" s="119" t="s">
+      <c r="D114" s="105"/>
+      <c r="E114" s="105"/>
+      <c r="F114" s="105"/>
+      <c r="G114" s="106"/>
+      <c r="H114" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="I114" s="121" t="s">
+      <c r="I114" s="108" t="s">
         <v>301</v>
       </c>
-      <c r="J114" s="121"/>
-      <c r="K114" s="119" t="s">
+      <c r="J114" s="108"/>
+      <c r="K114" s="106" t="s">
         <v>360</v>
       </c>
       <c r="L114" s="73"/>
@@ -17915,21 +17986,21 @@
       <c r="B115">
         <v>7</v>
       </c>
-      <c r="C115" s="114" t="s">
+      <c r="C115" s="101" t="s">
         <v>440</v>
       </c>
-      <c r="D115" s="118"/>
-      <c r="E115" s="118"/>
-      <c r="F115" s="118"/>
-      <c r="G115" s="119"/>
-      <c r="H115" s="119" t="s">
+      <c r="D115" s="105"/>
+      <c r="E115" s="105"/>
+      <c r="F115" s="105"/>
+      <c r="G115" s="106"/>
+      <c r="H115" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="I115" s="121" t="s">
+      <c r="I115" s="108" t="s">
         <v>302</v>
       </c>
-      <c r="J115" s="121"/>
-      <c r="K115" s="119" t="s">
+      <c r="J115" s="108"/>
+      <c r="K115" s="106" t="s">
         <v>360</v>
       </c>
       <c r="L115" s="73"/>
@@ -17942,21 +18013,21 @@
       <c r="B116">
         <v>8</v>
       </c>
-      <c r="C116" s="114" t="s">
+      <c r="C116" s="101" t="s">
         <v>441</v>
       </c>
-      <c r="D116" s="118"/>
-      <c r="E116" s="118"/>
-      <c r="F116" s="118"/>
-      <c r="G116" s="119"/>
-      <c r="H116" s="119" t="s">
+      <c r="D116" s="105"/>
+      <c r="E116" s="105"/>
+      <c r="F116" s="105"/>
+      <c r="G116" s="106"/>
+      <c r="H116" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="I116" s="121" t="s">
+      <c r="I116" s="108" t="s">
         <v>300</v>
       </c>
-      <c r="J116" s="121"/>
-      <c r="K116" s="119" t="s">
+      <c r="J116" s="108"/>
+      <c r="K116" s="106" t="s">
         <v>360</v>
       </c>
       <c r="L116" s="72"/>
@@ -17969,23 +18040,23 @@
       <c r="B117">
         <v>26</v>
       </c>
-      <c r="C117" s="114" t="s">
+      <c r="C117" s="101" t="s">
         <v>442</v>
       </c>
-      <c r="D117" s="118"/>
-      <c r="E117" s="118"/>
-      <c r="F117" s="118"/>
-      <c r="G117" s="119" t="s">
+      <c r="D117" s="105"/>
+      <c r="E117" s="105"/>
+      <c r="F117" s="105"/>
+      <c r="G117" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="H117" s="119" t="s">
+      <c r="H117" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="I117" s="121" t="s">
+      <c r="I117" s="108" t="s">
         <v>250</v>
       </c>
-      <c r="J117" s="121"/>
-      <c r="K117" s="119" t="s">
+      <c r="J117" s="108"/>
+      <c r="K117" s="106" t="s">
         <v>360</v>
       </c>
       <c r="L117" s="41"/>
@@ -17998,23 +18069,23 @@
       <c r="B118">
         <v>27</v>
       </c>
-      <c r="C118" s="114" t="s">
+      <c r="C118" s="101" t="s">
         <v>443</v>
       </c>
-      <c r="D118" s="118"/>
-      <c r="E118" s="118"/>
-      <c r="F118" s="118"/>
-      <c r="G118" s="119" t="s">
+      <c r="D118" s="105"/>
+      <c r="E118" s="105"/>
+      <c r="F118" s="105"/>
+      <c r="G118" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="H118" s="119" t="s">
+      <c r="H118" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="I118" s="121" t="s">
+      <c r="I118" s="108" t="s">
         <v>251</v>
       </c>
-      <c r="J118" s="121"/>
-      <c r="K118" s="119" t="s">
+      <c r="J118" s="108"/>
+      <c r="K118" s="106" t="s">
         <v>360</v>
       </c>
       <c r="L118" s="41"/>
@@ -18288,13 +18359,13 @@
       </c>
       <c r="D127" s="20"/>
       <c r="E127" s="20"/>
-      <c r="F127" s="98" t="s">
+      <c r="F127" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="G127" s="96" t="s">
+      <c r="G127" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="H127" s="94" t="s">
+      <c r="H127" s="112" t="s">
         <v>314</v>
       </c>
       <c r="I127" s="22" t="s">
@@ -18306,7 +18377,7 @@
       <c r="K127" s="19" t="s">
         <v>360</v>
       </c>
-      <c r="L127" s="92" t="s">
+      <c r="L127" s="110" t="s">
         <v>313</v>
       </c>
       <c r="M127" s="6"/>
@@ -18324,9 +18395,9 @@
       </c>
       <c r="D128" s="20"/>
       <c r="E128" s="20"/>
-      <c r="F128" s="99"/>
-      <c r="G128" s="97"/>
-      <c r="H128" s="95"/>
+      <c r="F128" s="117"/>
+      <c r="G128" s="115"/>
+      <c r="H128" s="113"/>
       <c r="I128" s="22" t="s">
         <v>378</v>
       </c>
@@ -18336,7 +18407,7 @@
       <c r="K128" s="19" t="s">
         <v>360</v>
       </c>
-      <c r="L128" s="93"/>
+      <c r="L128" s="111"/>
       <c r="M128" s="6"/>
     </row>
     <row r="129" spans="1:13" ht="26.25">
@@ -18403,7 +18474,7 @@
       <c r="J130" s="89" t="s">
         <v>375</v>
       </c>
-      <c r="K130" s="112" t="s">
+      <c r="K130" s="99" t="s">
         <v>360</v>
       </c>
       <c r="L130" s="90"/>
@@ -18692,39 +18763,39 @@
   </sheetData>
   <dataConsolidate/>
   <customSheetViews>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" scale="115">
+    <customSheetView guid="{984FFA58-0E1E-44C9-A906-B9154475911A}" scale="115" topLeftCell="F1">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L126" sqref="L126"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}" scale="115">
       <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L127" sqref="L127:L128"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-    </customSheetView>
-    <customSheetView guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}" scale="115">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+    <customSheetView guid="{3C568D49-0283-4011-B94D-E411C6036403}">
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H130" sqref="H130"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" scale="115">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" scale="115">
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" scale="115">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
     </customSheetView>
@@ -18734,35 +18805,41 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
     </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" scale="115">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
     </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" scale="115">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
     </customSheetView>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" scale="115">
+    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
     </customSheetView>
-    <customSheetView guid="{3C568D49-0283-4011-B94D-E411C6036403}">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H130" sqref="H130"/>
+    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
     </customSheetView>
-    <customSheetView guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}" scale="115">
+    <customSheetView guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}" scale="115">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+    </customSheetView>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" scale="115">
       <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L127" sqref="L127:L128"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
@@ -18894,7 +18971,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -18904,7 +18981,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -18945,15 +19022,15 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="100" t="s">
         <v>448</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
       <c r="E2" s="80" t="s">
         <v>436</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="100" t="s">
         <v>423</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -18986,15 +19063,15 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="100" t="s">
         <v>448</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="6"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
       <c r="E3" s="80" t="s">
         <v>422</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="100" t="s">
         <v>425</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -19027,15 +19104,19 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="100" t="s">
         <v>450</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="100">
+        <v>3488</v>
+      </c>
+      <c r="D4" s="100" t="s">
+        <v>451</v>
+      </c>
       <c r="E4" s="80" t="s">
         <v>427</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="100" t="s">
         <v>428</v>
       </c>
       <c r="G4" s="6" t="s">
@@ -19064,19 +19145,23 @@
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
     </row>
-    <row r="5" spans="1:29" ht="12.75">
+    <row r="5" spans="1:29" ht="25.5">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="100" t="s">
         <v>449</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
+      <c r="C5" s="100">
+        <v>3548</v>
+      </c>
+      <c r="D5" s="100" t="s">
+        <v>452</v>
+      </c>
       <c r="E5" s="80" t="s">
         <v>430</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="100" t="s">
         <v>431</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -19109,15 +19194,15 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="100" t="s">
         <v>448</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
       <c r="E6" s="80" t="s">
         <v>433</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="100" t="s">
         <v>435</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -19146,18 +19231,23 @@
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="1:29" ht="12.75">
+    <row r="7" spans="1:29" ht="25.5">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="113" t="s">
+      <c r="B7" s="100" t="s">
         <v>449</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="100">
+        <v>3549</v>
+      </c>
+      <c r="D7" s="78" t="s">
+        <v>453</v>
+      </c>
       <c r="E7" s="80" t="s">
         <v>445</v>
       </c>
-      <c r="F7" s="120" t="s">
+      <c r="F7" s="107" t="s">
         <v>446</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -20313,19 +20403,49 @@
     <row r="44" spans="1:29" ht="38.25" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
+    <customSheetView guid="{984FFA58-0E1E-44C9-A906-B9154475911A}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-    </customSheetView>
-    <customSheetView guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+    <customSheetView guid="{3C568D49-0283-4011-B94D-E411C6036403}">
+      <selection activeCell="B14" sqref="B14"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+    </customSheetView>
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20335,50 +20455,26 @@
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
+    <customSheetView guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{3C568D49-0283-4011-B94D-E411C6036403}">
-      <selection activeCell="B14" sqref="B14"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-    </customSheetView>
-    <customSheetView guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}">
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -20453,7 +20549,7 @@
         <v>171</v>
       </c>
       <c r="I2" s="8"/>
-      <c r="J2" s="107"/>
+      <c r="J2" s="94"/>
     </row>
     <row r="3" spans="1:10" ht="30">
       <c r="A3">
@@ -20476,7 +20572,7 @@
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="107"/>
+      <c r="J3" s="94"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4">
@@ -20499,7 +20595,7 @@
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="107"/>
+      <c r="J4" s="94"/>
     </row>
     <row r="5" spans="1:10" ht="15">
       <c r="A5">
@@ -20522,7 +20618,7 @@
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="12"/>
-      <c r="J5" s="107"/>
+      <c r="J5" s="94"/>
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6">
@@ -20545,7 +20641,7 @@
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="12"/>
-      <c r="J6" s="107"/>
+      <c r="J6" s="94"/>
     </row>
     <row r="7" spans="1:10" ht="15">
       <c r="A7">
@@ -20568,7 +20664,7 @@
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="12"/>
-      <c r="J7" s="107"/>
+      <c r="J7" s="94"/>
     </row>
     <row r="8" spans="1:10" ht="30">
       <c r="A8">
@@ -20591,7 +20687,7 @@
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="108" t="s">
+      <c r="J8" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -20616,7 +20712,7 @@
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="105" t="s">
+      <c r="J9" s="92" t="s">
         <v>360</v>
       </c>
     </row>
@@ -20643,7 +20739,7 @@
         <v>213</v>
       </c>
       <c r="I10" s="8"/>
-      <c r="J10" s="105" t="s">
+      <c r="J10" s="92" t="s">
         <v>360</v>
       </c>
     </row>
@@ -20670,7 +20766,7 @@
         <v>214</v>
       </c>
       <c r="I11" s="8"/>
-      <c r="J11" s="105" t="s">
+      <c r="J11" s="92" t="s">
         <v>360</v>
       </c>
     </row>
@@ -20695,7 +20791,7 @@
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="107"/>
+      <c r="J12" s="94"/>
     </row>
     <row r="13" spans="1:10" ht="15">
       <c r="A13">
@@ -20718,7 +20814,7 @@
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="107"/>
+      <c r="J13" s="94"/>
     </row>
     <row r="14" spans="1:10" ht="15">
       <c r="A14">
@@ -20741,7 +20837,7 @@
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="107"/>
+      <c r="J14" s="94"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15">
@@ -20764,7 +20860,7 @@
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="107"/>
+      <c r="J15" s="94"/>
     </row>
     <row r="16" spans="1:10" ht="15">
       <c r="A16">
@@ -20787,7 +20883,7 @@
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="107"/>
+      <c r="J16" s="94"/>
     </row>
     <row r="17" spans="1:10" ht="15">
       <c r="A17">
@@ -20810,7 +20906,7 @@
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="107"/>
+      <c r="J17" s="94"/>
     </row>
     <row r="18" spans="1:10" ht="30">
       <c r="A18">
@@ -20833,7 +20929,7 @@
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="107"/>
+      <c r="J18" s="94"/>
     </row>
     <row r="19" spans="1:10" ht="15">
       <c r="A19">
@@ -20856,7 +20952,7 @@
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
-      <c r="J19" s="107"/>
+      <c r="J19" s="94"/>
     </row>
     <row r="20" spans="1:10" ht="39">
       <c r="A20">
@@ -20879,7 +20975,7 @@
       </c>
       <c r="H20" s="32"/>
       <c r="I20" s="32"/>
-      <c r="J20" s="107"/>
+      <c r="J20" s="94"/>
     </row>
     <row r="21" spans="1:10" ht="39">
       <c r="A21">
@@ -20902,7 +20998,7 @@
       </c>
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
-      <c r="J21" s="107"/>
+      <c r="J21" s="94"/>
     </row>
     <row r="22" spans="1:10" s="53" customFormat="1" ht="39">
       <c r="A22" s="53">
@@ -20927,7 +21023,7 @@
       </c>
       <c r="H22" s="23"/>
       <c r="I22" s="65"/>
-      <c r="J22" s="107"/>
+      <c r="J22" s="94"/>
     </row>
     <row r="23" spans="1:10" ht="15">
       <c r="A23">
@@ -20950,7 +21046,7 @@
       </c>
       <c r="H23" s="33"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="107"/>
+      <c r="J23" s="94"/>
     </row>
     <row r="24" spans="1:10" ht="15">
       <c r="A24">
@@ -20973,7 +21069,7 @@
       </c>
       <c r="H24" s="33"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="107"/>
+      <c r="J24" s="94"/>
     </row>
     <row r="25" spans="1:10" ht="15">
       <c r="A25">
@@ -20996,7 +21092,7 @@
       </c>
       <c r="H25" s="33"/>
       <c r="I25" s="11"/>
-      <c r="J25" s="107"/>
+      <c r="J25" s="94"/>
     </row>
     <row r="26" spans="1:10" ht="15">
       <c r="A26">
@@ -21019,7 +21115,7 @@
       </c>
       <c r="H26" s="33"/>
       <c r="I26" s="8"/>
-      <c r="J26" s="107"/>
+      <c r="J26" s="94"/>
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27">
@@ -21042,7 +21138,7 @@
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="12"/>
-      <c r="J27" s="107"/>
+      <c r="J27" s="94"/>
     </row>
     <row r="28" spans="1:10" ht="15">
       <c r="A28">
@@ -21065,7 +21161,7 @@
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
-      <c r="J28" s="107"/>
+      <c r="J28" s="94"/>
     </row>
     <row r="29" spans="1:10" ht="15">
       <c r="A29">
@@ -21088,7 +21184,7 @@
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
-      <c r="J29" s="107"/>
+      <c r="J29" s="94"/>
     </row>
     <row r="30" spans="1:10" ht="15">
       <c r="A30">
@@ -21111,7 +21207,7 @@
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
-      <c r="J30" s="107"/>
+      <c r="J30" s="94"/>
     </row>
     <row r="31" spans="1:10" ht="15">
       <c r="A31">
@@ -21134,7 +21230,7 @@
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="107"/>
+      <c r="J31" s="94"/>
     </row>
     <row r="32" spans="1:10" ht="15">
       <c r="A32">
@@ -21157,7 +21253,7 @@
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
-      <c r="J32" s="122" t="s">
+      <c r="J32" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21182,7 +21278,7 @@
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="122" t="s">
+      <c r="J33" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21209,7 +21305,7 @@
         <v>173</v>
       </c>
       <c r="I34" s="8"/>
-      <c r="J34" s="122" t="s">
+      <c r="J34" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21236,7 +21332,7 @@
         <v>174</v>
       </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="122" t="s">
+      <c r="J35" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21263,7 +21359,7 @@
         <v>178</v>
       </c>
       <c r="I36" s="8"/>
-      <c r="J36" s="122" t="s">
+      <c r="J36" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21290,7 +21386,7 @@
         <v>179</v>
       </c>
       <c r="I37" s="8"/>
-      <c r="J37" s="122" t="s">
+      <c r="J37" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21317,7 +21413,7 @@
         <v>182</v>
       </c>
       <c r="I38" s="8"/>
-      <c r="J38" s="122" t="s">
+      <c r="J38" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21342,7 +21438,7 @@
       </c>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
-      <c r="J39" s="122" t="s">
+      <c r="J39" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21367,7 +21463,7 @@
       </c>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
-      <c r="J40" s="122" t="s">
+      <c r="J40" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21393,7 +21489,7 @@
       </c>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
-      <c r="J41" s="122" t="s">
+      <c r="J41" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21418,7 +21514,7 @@
       </c>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
-      <c r="J42" s="122" t="s">
+      <c r="J42" s="109" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21443,7 +21539,7 @@
       </c>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
-      <c r="J43" s="107"/>
+      <c r="J43" s="94"/>
     </row>
     <row r="44" spans="1:10" ht="15">
       <c r="A44">
@@ -21466,7 +21562,7 @@
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
-      <c r="J44" s="107"/>
+      <c r="J44" s="94"/>
     </row>
     <row r="45" spans="1:10" ht="15">
       <c r="A45">
@@ -21489,7 +21585,7 @@
       </c>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
-      <c r="J45" s="107"/>
+      <c r="J45" s="94"/>
     </row>
     <row r="46" spans="1:10" ht="15">
       <c r="A46">
@@ -21512,7 +21608,7 @@
       </c>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
-      <c r="J46" s="107"/>
+      <c r="J46" s="94"/>
     </row>
     <row r="47" spans="1:10" ht="15">
       <c r="A47">
@@ -21535,7 +21631,7 @@
       </c>
       <c r="H47" s="8"/>
       <c r="I47" s="11"/>
-      <c r="J47" s="107"/>
+      <c r="J47" s="94"/>
     </row>
     <row r="48" spans="1:10" ht="15">
       <c r="A48">
@@ -21558,7 +21654,7 @@
       </c>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
-      <c r="J48" s="107"/>
+      <c r="J48" s="94"/>
     </row>
     <row r="49" spans="1:10" ht="15">
       <c r="A49">
@@ -21581,7 +21677,7 @@
       </c>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
-      <c r="J49" s="107"/>
+      <c r="J49" s="94"/>
     </row>
     <row r="50" spans="1:10" ht="15">
       <c r="A50">
@@ -21604,7 +21700,7 @@
       </c>
       <c r="H50" s="33"/>
       <c r="I50" s="8"/>
-      <c r="J50" s="107"/>
+      <c r="J50" s="94"/>
     </row>
     <row r="51" spans="1:10" ht="15">
       <c r="A51">
@@ -21627,7 +21723,7 @@
       </c>
       <c r="H51" s="33"/>
       <c r="I51" s="8"/>
-      <c r="J51" s="107"/>
+      <c r="J51" s="94"/>
     </row>
     <row r="52" spans="1:10" ht="15">
       <c r="A52">
@@ -21650,7 +21746,7 @@
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
-      <c r="J52" s="107"/>
+      <c r="J52" s="94"/>
     </row>
     <row r="53" spans="1:10" ht="15">
       <c r="A53">
@@ -21673,7 +21769,7 @@
       </c>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
-      <c r="J53" s="107"/>
+      <c r="J53" s="94"/>
     </row>
     <row r="54" spans="1:10" ht="15">
       <c r="A54">
@@ -21696,7 +21792,7 @@
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
-      <c r="J54" s="107"/>
+      <c r="J54" s="94"/>
     </row>
     <row r="55" spans="1:10" ht="15">
       <c r="A55">
@@ -21719,7 +21815,7 @@
       </c>
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
-      <c r="J55" s="107"/>
+      <c r="J55" s="94"/>
     </row>
     <row r="56" spans="1:10" ht="30">
       <c r="A56">
@@ -21744,7 +21840,7 @@
       <c r="I56" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="J56" s="107"/>
+      <c r="J56" s="94"/>
     </row>
     <row r="57" spans="1:10" ht="15">
       <c r="A57">
@@ -21767,7 +21863,7 @@
       </c>
       <c r="H57" s="20"/>
       <c r="I57" s="63"/>
-      <c r="J57" s="107"/>
+      <c r="J57" s="94"/>
     </row>
     <row r="58" spans="1:10" ht="26.25">
       <c r="A58">
@@ -21792,7 +21888,7 @@
         <v>257</v>
       </c>
       <c r="I58" s="65"/>
-      <c r="J58" s="107"/>
+      <c r="J58" s="94"/>
     </row>
     <row r="59" spans="1:10" ht="15">
       <c r="A59">
@@ -21815,7 +21911,7 @@
       </c>
       <c r="H59" s="42"/>
       <c r="I59" s="64"/>
-      <c r="J59" s="107"/>
+      <c r="J59" s="94"/>
     </row>
     <row r="60" spans="1:10" ht="26.25">
       <c r="A60">
@@ -21838,7 +21934,7 @@
       </c>
       <c r="H60" s="42"/>
       <c r="I60" s="64"/>
-      <c r="J60" s="107"/>
+      <c r="J60" s="94"/>
     </row>
     <row r="61" spans="1:10" ht="26.25">
       <c r="A61">
@@ -21861,7 +21957,7 @@
       </c>
       <c r="H61" s="42"/>
       <c r="I61" s="64"/>
-      <c r="J61" s="107"/>
+      <c r="J61" s="94"/>
     </row>
     <row r="62" spans="1:10" ht="15">
       <c r="A62">
@@ -21884,7 +21980,7 @@
       </c>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
-      <c r="J62" s="108" t="s">
+      <c r="J62" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21909,7 +22005,7 @@
       </c>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
-      <c r="J63" s="108" t="s">
+      <c r="J63" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21934,7 +22030,7 @@
       </c>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
-      <c r="J64" s="108" t="s">
+      <c r="J64" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21959,7 +22055,7 @@
       </c>
       <c r="H65" s="8"/>
       <c r="I65" s="8"/>
-      <c r="J65" s="108" t="s">
+      <c r="J65" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -21984,7 +22080,7 @@
       </c>
       <c r="H66" s="8"/>
       <c r="I66" s="8"/>
-      <c r="J66" s="108" t="s">
+      <c r="J66" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -22009,7 +22105,7 @@
       </c>
       <c r="H67" s="8"/>
       <c r="I67" s="8"/>
-      <c r="J67" s="108" t="s">
+      <c r="J67" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -22034,7 +22130,7 @@
       </c>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
-      <c r="J68" s="108" t="s">
+      <c r="J68" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -22059,7 +22155,7 @@
       </c>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
-      <c r="J69" s="108" t="s">
+      <c r="J69" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -22084,7 +22180,7 @@
       </c>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
-      <c r="J70" s="108" t="s">
+      <c r="J70" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -22109,7 +22205,7 @@
       </c>
       <c r="H71" s="28"/>
       <c r="I71" s="28"/>
-      <c r="J71" s="108" t="s">
+      <c r="J71" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -22134,7 +22230,7 @@
       </c>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
-      <c r="J72" s="108" t="s">
+      <c r="J72" s="95" t="s">
         <v>360</v>
       </c>
     </row>
@@ -22159,7 +22255,7 @@
       </c>
       <c r="H73" s="8"/>
       <c r="I73" s="11"/>
-      <c r="J73" s="107"/>
+      <c r="J73" s="94"/>
     </row>
     <row r="74" spans="1:10" ht="15">
       <c r="A74">
@@ -22182,7 +22278,7 @@
       </c>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
-      <c r="J74" s="107"/>
+      <c r="J74" s="94"/>
     </row>
     <row r="75" spans="1:10" ht="15">
       <c r="A75">
@@ -22205,7 +22301,7 @@
       </c>
       <c r="H75" s="8"/>
       <c r="I75" s="8"/>
-      <c r="J75" s="107"/>
+      <c r="J75" s="94"/>
     </row>
     <row r="76" spans="1:10" ht="15">
       <c r="A76">
@@ -22228,7 +22324,7 @@
       </c>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
-      <c r="J76" s="107"/>
+      <c r="J76" s="94"/>
     </row>
     <row r="77" spans="1:10" ht="15">
       <c r="A77">
@@ -22251,7 +22347,7 @@
       </c>
       <c r="H77" s="8"/>
       <c r="I77" s="8"/>
-      <c r="J77" s="107"/>
+      <c r="J77" s="94"/>
     </row>
     <row r="78" spans="1:10" ht="15">
       <c r="A78">
@@ -22274,7 +22370,7 @@
       </c>
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
-      <c r="J78" s="107"/>
+      <c r="J78" s="94"/>
     </row>
     <row r="79" spans="1:10" ht="26.25">
       <c r="A79">
@@ -22297,7 +22393,7 @@
       </c>
       <c r="H79" s="12"/>
       <c r="I79" s="12"/>
-      <c r="J79" s="107"/>
+      <c r="J79" s="94"/>
     </row>
     <row r="80" spans="1:10" ht="26.25">
       <c r="A80">
@@ -22322,7 +22418,7 @@
       <c r="I80" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J80" s="107"/>
+      <c r="J80" s="94"/>
     </row>
     <row r="81" spans="1:10" ht="26.25">
       <c r="A81">
@@ -22347,7 +22443,7 @@
       <c r="I81" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J81" s="107"/>
+      <c r="J81" s="94"/>
     </row>
     <row r="82" spans="1:10" ht="26.25">
       <c r="A82">
@@ -22372,7 +22468,7 @@
       <c r="I82" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J82" s="107"/>
+      <c r="J82" s="94"/>
     </row>
     <row r="83" spans="1:10" ht="26.25">
       <c r="A83">
@@ -22397,7 +22493,7 @@
       <c r="I83" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J83" s="107"/>
+      <c r="J83" s="94"/>
     </row>
     <row r="84" spans="1:10" ht="26.25">
       <c r="A84">
@@ -22422,7 +22518,7 @@
       <c r="I84" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J84" s="107"/>
+      <c r="J84" s="94"/>
     </row>
     <row r="85" spans="1:10" ht="26.25">
       <c r="A85">
@@ -22447,7 +22543,7 @@
       <c r="I85" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J85" s="107"/>
+      <c r="J85" s="94"/>
     </row>
     <row r="86" spans="1:10" ht="26.25">
       <c r="A86">
@@ -22472,7 +22568,7 @@
       <c r="I86" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J86" s="107"/>
+      <c r="J86" s="94"/>
     </row>
     <row r="87" spans="1:10" ht="26.25">
       <c r="A87">
@@ -22497,7 +22593,7 @@
       <c r="I87" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J87" s="107"/>
+      <c r="J87" s="94"/>
     </row>
     <row r="88" spans="1:10" ht="26.25">
       <c r="A88">
@@ -22522,7 +22618,7 @@
       <c r="I88" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J88" s="107"/>
+      <c r="J88" s="94"/>
     </row>
     <row r="89" spans="1:10" ht="26.25">
       <c r="A89">
@@ -22547,7 +22643,7 @@
       <c r="I89" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J89" s="107"/>
+      <c r="J89" s="94"/>
     </row>
     <row r="90" spans="1:10" ht="26.25">
       <c r="A90">
@@ -22572,7 +22668,7 @@
       <c r="I90" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J90" s="107"/>
+      <c r="J90" s="94"/>
     </row>
     <row r="91" spans="1:10" ht="26.25">
       <c r="A91">
@@ -22597,7 +22693,7 @@
       <c r="I91" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J91" s="107"/>
+      <c r="J91" s="94"/>
     </row>
     <row r="92" spans="1:10" ht="26.25">
       <c r="A92">
@@ -22622,7 +22718,7 @@
       <c r="I92" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J92" s="107"/>
+      <c r="J92" s="94"/>
     </row>
     <row r="93" spans="1:10" ht="26.25">
       <c r="A93">
@@ -22647,7 +22743,7 @@
       <c r="I93" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J93" s="107"/>
+      <c r="J93" s="94"/>
     </row>
     <row r="94" spans="1:10" ht="26.25">
       <c r="A94">
@@ -22672,7 +22768,7 @@
       <c r="I94" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J94" s="107"/>
+      <c r="J94" s="94"/>
     </row>
     <row r="95" spans="1:10" ht="26.25">
       <c r="A95">
@@ -22697,7 +22793,7 @@
       <c r="I95" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J95" s="107"/>
+      <c r="J95" s="94"/>
     </row>
     <row r="96" spans="1:10" ht="26.25">
       <c r="A96" s="66">
@@ -22722,23 +22818,31 @@
       <c r="I96" s="70" t="s">
         <v>183</v>
       </c>
-      <c r="J96" s="107"/>
+      <c r="J96" s="94"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
+    <customSheetView guid="{984FFA58-0E1E-44C9-A906-B9154475911A}" topLeftCell="A10">
+      <selection activeCell="I43" sqref="I43"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}">
       <selection activeCell="G80" sqref="G80"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}" topLeftCell="A82">
+    <customSheetView guid="{3C568D49-0283-4011-B94D-E411C6036403}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" topLeftCell="A82">
       <selection activeCell="F113" sqref="F113"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" topLeftCell="A4">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" topLeftCell="A13">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" topLeftCell="A4">
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
       <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -22746,28 +22850,25 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" topLeftCell="A4">
       <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" topLeftCell="A13">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" topLeftCell="A4">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" topLeftCell="A82">
+    <customSheetView guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}" topLeftCell="A82">
       <selection activeCell="F113" sqref="F113"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3C568D49-0283-4011-B94D-E411C6036403}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}">
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
       <selection activeCell="G80" sqref="G80"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -22782,35 +22883,39 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
+    <customSheetView guid="{984FFA58-0E1E-44C9-A906-B9154475911A}">
       <selection activeCell="J26" sqref="J26"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}">
+      <selection activeCell="J26" sqref="J26"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{3C568D49-0283-4011-B94D-E411C6036403}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{7673B41A-DE25-4D70-9D35-C78C1B37CB7D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{3C568D49-0283-4011-B94D-E411C6036403}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{D94C77A3-4647-4E88-B8DA-2D06EDBBF681}">
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
       <selection activeCell="J26" sqref="J26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>